<commit_message>
update thong ke nguong
</commit_message>
<xml_diff>
--- a/ThongKeNguong.xlsx
+++ b/ThongKeNguong.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Class\ky2_2122\XL tín hiệu số\Handle speech signal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D65E7-5679-4772-B7DB-2CE936F267AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F295D7B0-A7A8-4C83-A624-636D9CCD7F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B47E6B4-FF19-4334-8229-3A9AFBCD530A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{4B47E6B4-FF19-4334-8229-3A9AFBCD530A}"/>
   </bookViews>
   <sheets>
     <sheet name="Studio" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="17">
   <si>
     <t>Studio_female</t>
   </si>
@@ -64,16 +71,19 @@
     <t>Voice</t>
   </si>
   <si>
-    <t>0.3 -&gt; 0.32</t>
-  </si>
-  <si>
     <t xml:space="preserve">Voice </t>
   </si>
   <si>
-    <t>0.28 -&gt; 0.3</t>
+    <t>0.29 - &gt; 0.3</t>
   </si>
   <si>
-    <t>0.3 -&gt; 0.33</t>
+    <t>0.28 -&gt; 0.36( chọn 0.3)</t>
+  </si>
+  <si>
+    <t>0.28 -&gt; 0.38(chọn 0.3)</t>
+  </si>
+  <si>
+    <t>0.3 -&gt; 0.38(chọn 0.3)</t>
   </si>
 </sst>
 </file>
@@ -109,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -126,6 +136,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF5C30D-5A8E-4793-A983-56FBF19A73A6}">
   <dimension ref="A1:S143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100:C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -521,7 +534,8 @@
         <v>0.44444444444444436</v>
       </c>
       <c r="E3">
-        <v>0.44</v>
+        <f xml:space="preserve"> MIN(D3:D24)</f>
+        <v>0.18390804597701152</v>
       </c>
       <c r="F3">
         <v>1E-4</v>
@@ -535,6 +549,10 @@
       <c r="I3">
         <f xml:space="preserve"> G3 / F3</f>
         <v>1</v>
+      </c>
+      <c r="J3">
+        <f xml:space="preserve"> MIN(I3:I21,I22:I30)</f>
+        <v>0.2</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1316,7 +1334,7 @@
         <v>0.56283185840707961</v>
       </c>
       <c r="E25">
-        <v>0.56000000000000005</v>
+        <v>0.562832</v>
       </c>
       <c r="F25">
         <v>4.1000000000000003E-3</v>
@@ -1355,7 +1373,8 @@
         <v>0.26076285918805603</v>
       </c>
       <c r="E26">
-        <v>0.26</v>
+        <f xml:space="preserve"> MAX(D26:D38)</f>
+        <v>0.34226009332521806</v>
       </c>
       <c r="F26">
         <v>4.1000000000000003E-3</v>
@@ -1550,6 +1569,10 @@
         <f t="shared" si="1"/>
         <v>0.35820895522388058</v>
       </c>
+      <c r="J31">
+        <f xml:space="preserve"> MIN(I31:I33)</f>
+        <v>0.35820895522388058</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1658,6 +1681,10 @@
         <f t="shared" si="1"/>
         <v>0.36320000000000002</v>
       </c>
+      <c r="J34">
+        <f xml:space="preserve"> MAX(I34:I44)</f>
+        <v>0.36320000000000002</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -1826,7 +1853,8 @@
         <v>0.38675213675213677</v>
       </c>
       <c r="E39">
-        <v>0.43</v>
+        <f xml:space="preserve"> MIN(D39,D40)</f>
+        <v>0.38675213675213677</v>
       </c>
       <c r="F39">
         <v>0.38319999999999999</v>
@@ -1901,7 +1929,8 @@
         <v>0.23209418946909408</v>
       </c>
       <c r="E41">
-        <v>0.24</v>
+        <f xml:space="preserve"> MAX(D41:D42)</f>
+        <v>0.24684542586750791</v>
       </c>
       <c r="F41">
         <v>0.3513</v>
@@ -1976,7 +2005,8 @@
         <v>0.40259740259740262</v>
       </c>
       <c r="E43">
-        <v>0.56000000000000005</v>
+        <f>MIN(D43:D44)</f>
+        <v>0.40259740259740262</v>
       </c>
       <c r="F43">
         <v>0.35570000000000002</v>
@@ -2051,7 +2081,8 @@
         <v>0.15554708349218455</v>
       </c>
       <c r="E45">
-        <v>0.28999999999999998</v>
+        <f>MAX(D45:D56)</f>
+        <v>0.29365370506236244</v>
       </c>
       <c r="F45">
         <v>7.6300000000000007E-2</v>
@@ -2064,6 +2095,10 @@
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
+        <v>0.45478374836173002</v>
+      </c>
+      <c r="J45">
+        <f>MIN(I45:I46)</f>
         <v>0.45478374836173002</v>
       </c>
       <c r="K45" s="1"/>
@@ -2138,6 +2173,10 @@
         <f t="shared" si="1"/>
         <v>0.41096849474912489</v>
       </c>
+      <c r="J47">
+        <f xml:space="preserve"> MAX(I47:I55)</f>
+        <v>0.41096849474912489</v>
+      </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -2462,6 +2501,10 @@
         <f t="shared" si="1"/>
         <v>0.49911504424778758</v>
       </c>
+      <c r="J56">
+        <f xml:space="preserve"> MIN(I56:I57)</f>
+        <v>0.4349298500241896</v>
+      </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -2486,7 +2529,8 @@
         <v>0.35432750914262495</v>
       </c>
       <c r="E57">
-        <v>0.54</v>
+        <f xml:space="preserve"> MIN(D57:D58)</f>
+        <v>0.35432750914262495</v>
       </c>
       <c r="F57">
         <v>0.20669999999999999</v>
@@ -2537,6 +2581,10 @@
         <f t="shared" si="1"/>
         <v>0.44811320754716982</v>
       </c>
+      <c r="J58">
+        <f xml:space="preserve"> MAX(I58:I61)</f>
+        <v>0.48837209302325579</v>
+      </c>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -2561,7 +2609,8 @@
         <v>0.52266820675714698</v>
       </c>
       <c r="E59">
-        <v>0.52</v>
+        <f xml:space="preserve"> MAX(D59:D60)</f>
+        <v>0.52266820675714698</v>
       </c>
       <c r="F59">
         <v>0.37580000000000002</v>
@@ -2635,6 +2684,9 @@
         <f t="shared" si="0"/>
         <v>0.47719030349303299</v>
       </c>
+      <c r="E61">
+        <v>0.47719</v>
+      </c>
       <c r="F61">
         <v>1.95E-2</v>
       </c>
@@ -2672,7 +2724,8 @@
         <v>0.53474903474903479</v>
       </c>
       <c r="E62">
-        <v>0.53</v>
+        <f>MAX(D62:D64)</f>
+        <v>0.53474903474903479</v>
       </c>
       <c r="F62">
         <v>1.77E-2</v>
@@ -2685,6 +2738,10 @@
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
+        <v>0.20338983050847456</v>
+      </c>
+      <c r="J62">
+        <f xml:space="preserve"> MIN(I62:I63)</f>
         <v>0.20338983050847456</v>
       </c>
       <c r="K62" s="1"/>
@@ -2759,6 +2816,10 @@
         <f t="shared" si="1"/>
         <v>0.28077651515151514</v>
       </c>
+      <c r="J64">
+        <f xml:space="preserve"> MAX(I64:I70)</f>
+        <v>0.28077651515151514</v>
+      </c>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -2783,7 +2844,8 @@
         <v>0.53260869565217395</v>
       </c>
       <c r="E65">
-        <v>0.53</v>
+        <f>MIN(D65:D67)</f>
+        <v>0.33485580060028708</v>
       </c>
       <c r="F65">
         <v>0.48880000000000001</v>
@@ -2894,7 +2956,8 @@
         <v>0.12218116957574213</v>
       </c>
       <c r="E68">
-        <v>0.14000000000000001</v>
+        <f xml:space="preserve"> MAX(D68:D73)</f>
+        <v>0.14203854835909013</v>
       </c>
       <c r="F68">
         <v>0.27850000000000003</v>
@@ -3017,6 +3080,10 @@
         <f t="shared" si="3"/>
         <v>0.36951983298538627</v>
       </c>
+      <c r="J71">
+        <f xml:space="preserve"> MIN(I71:I91,I92:I93)</f>
+        <v>0.23076923076923075</v>
+      </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -3113,7 +3180,8 @@
         <v>0.31349206349206354</v>
       </c>
       <c r="E74">
-        <v>0.72</v>
+        <f xml:space="preserve"> MIN(D74,D75,D76,D77,D78,D79,D80,D81,D82,D83,D84,D85,D86,D87,D88,D89,D90,D91,D92,D93,D94,D95,D96,D97)</f>
+        <v>0.31343283582089548</v>
       </c>
       <c r="F74">
         <v>9.7000000000000003E-3</v>
@@ -3934,18 +4002,21 @@
       <c r="S99" s="1"/>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B100">
-        <v>0.3</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="B100" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="7"/>
+      <c r="F100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G100" t="s">
-        <v>12</v>
-      </c>
+      <c r="G100" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
@@ -4382,10 +4453,12 @@
       <c r="S143" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="P143:S143"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="G100:I100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4394,15 +4467,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF1C9F2-E668-4C8F-9AA3-088A854E6FE4}">
-  <dimension ref="A1:I143"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="J143" sqref="J143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -4416,7 +4489,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4442,7 +4515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.49E-2</v>
       </c>
@@ -4456,6 +4529,10 @@
         <f xml:space="preserve"> B3 / A3</f>
         <v>0.51677852348993292</v>
       </c>
+      <c r="E3">
+        <f xml:space="preserve"> MIN(D3:D19)</f>
+        <v>0.42105263157894735</v>
+      </c>
       <c r="F3">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -4469,8 +4546,12 @@
         <f xml:space="preserve"> G3 / F3</f>
         <v>0.46666666666666667</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f xml:space="preserve"> MIN(I3:I18)</f>
+        <v>0.42723004694835681</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.38E-2</v>
       </c>
@@ -4498,7 +4579,7 @@
         <v>0.45049504950495056</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1.7399999999999999E-2</v>
       </c>
@@ -4526,7 +4607,7 @@
         <v>0.50802139037433147</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2.06E-2</v>
       </c>
@@ -4554,7 +4635,7 @@
         <v>0.56157635467980305</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.8100000000000002E-2</v>
       </c>
@@ -4582,7 +4663,7 @@
         <v>0.55172413793103448</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.7500000000000002E-2</v>
       </c>
@@ -4610,7 +4691,7 @@
         <v>0.42723004694835681</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.4E-2</v>
       </c>
@@ -4638,7 +4719,7 @@
         <v>0.47290640394088668</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1.7500000000000002E-2</v>
       </c>
@@ -4666,7 +4747,7 @@
         <v>0.50555555555555565</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.7100000000000001E-2</v>
       </c>
@@ -4694,7 +4775,7 @@
         <v>0.45495495495495492</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1.7100000000000001E-2</v>
       </c>
@@ -4722,7 +4803,7 @@
         <v>0.51724137931034486</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -4750,7 +4831,7 @@
         <v>0.60693641618497118</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1.84E-2</v>
       </c>
@@ -4778,7 +4859,7 @@
         <v>0.42738589211618255</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1.5800000000000002E-2</v>
       </c>
@@ -4806,7 +4887,7 @@
         <v>0.57425742574257421</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1.52E-2</v>
       </c>
@@ -4834,7 +4915,7 @@
         <v>0.53246753246753253</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.4800000000000001E-2</v>
       </c>
@@ -4862,7 +4943,7 @@
         <v>0.48947368421052628</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1.6899999999999998E-2</v>
       </c>
@@ -4890,7 +4971,7 @@
         <v>0.53012048192771088</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1.8700000000000001E-2</v>
       </c>
@@ -4917,8 +4998,12 @@
         <f t="shared" si="1"/>
         <v>9.5480074886333255E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <f xml:space="preserve"> MAX(I19:I34,I35:I48)</f>
+        <v>0.4192662350402197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2.01E-2</v>
       </c>
@@ -4932,6 +5017,10 @@
         <f t="shared" si="0"/>
         <v>0.42786069651741293</v>
       </c>
+      <c r="E20">
+        <f xml:space="preserve"> MAX(D20:D38,D39:D40)</f>
+        <v>0.42786069651741293</v>
+      </c>
       <c r="F20">
         <v>0.51519999999999999</v>
       </c>
@@ -4946,7 +5035,7 @@
         <v>9.2197204968944096E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.27129999999999999</v>
       </c>
@@ -4974,7 +5063,7 @@
         <v>8.3178360101437018E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.47220000000000001</v>
       </c>
@@ -5002,7 +5091,7 @@
         <v>0.16906196878380467</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0.50629999999999997</v>
       </c>
@@ -5030,7 +5119,7 @@
         <v>0.11691348402182385</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0.81679999999999997</v>
       </c>
@@ -5058,7 +5147,7 @@
         <v>0.19611996878135801</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0.85909999999999997</v>
       </c>
@@ -5086,7 +5175,7 @@
         <v>0.24104356509799024</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.76929999999999998</v>
       </c>
@@ -5114,7 +5203,7 @@
         <v>0.1941169465285221</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0.64410000000000001</v>
       </c>
@@ -5142,7 +5231,7 @@
         <v>0.1372674791533034</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0.65639999999999998</v>
       </c>
@@ -5170,7 +5259,7 @@
         <v>0.14381487889273359</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0.36620000000000003</v>
       </c>
@@ -5198,7 +5287,7 @@
         <v>0.22460391425908666</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0.81010000000000004</v>
       </c>
@@ -5226,7 +5315,7 @@
         <v>0.27976190476190477</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0.83809999999999996</v>
       </c>
@@ -5254,7 +5343,7 @@
         <v>0.13500404203718674</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.68859999999999999</v>
       </c>
@@ -5520,6 +5609,10 @@
         <f t="shared" si="0"/>
         <v>0.4178082191780822</v>
       </c>
+      <c r="E41">
+        <f xml:space="preserve"> MIN(D41:D43)</f>
+        <v>0.40203850509626271</v>
+      </c>
       <c r="F41">
         <v>0.53180000000000005</v>
       </c>
@@ -5604,6 +5697,10 @@
         <f t="shared" si="0"/>
         <v>0.15271186440677967</v>
       </c>
+      <c r="E44">
+        <f xml:space="preserve"> MAX(D44:D47)</f>
+        <v>0.19952662721893491</v>
+      </c>
       <c r="F44">
         <v>0.31119999999999998</v>
       </c>
@@ -5716,6 +5813,10 @@
         <f t="shared" si="0"/>
         <v>0.51219512195121952</v>
       </c>
+      <c r="E48">
+        <f xml:space="preserve"> MIN(D48:D50)</f>
+        <v>0.40470297029702973</v>
+      </c>
       <c r="F48">
         <v>9.9099999999999994E-2</v>
       </c>
@@ -5730,7 +5831,7 @@
         <v>0.19677093844601415</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>3.4099999999999998E-2</v>
       </c>
@@ -5757,8 +5858,12 @@
         <f t="shared" si="1"/>
         <v>0.34986945169712796</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49">
+        <f xml:space="preserve"> MIN(I49:I52)</f>
+        <v>0.34986945169712796</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>8.0799999999999997E-2</v>
       </c>
@@ -5786,7 +5891,7 @@
         <v>0.54140127388535031</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0.27710000000000001</v>
       </c>
@@ -5800,6 +5905,10 @@
         <f t="shared" si="0"/>
         <v>0.44243955250811978</v>
       </c>
+      <c r="E51">
+        <f xml:space="preserve"> MAX(D51:D55)</f>
+        <v>0.44243955250811978</v>
+      </c>
       <c r="F51">
         <v>7.6300000000000007E-2</v>
       </c>
@@ -5814,7 +5923,7 @@
         <v>0.46002621231979024</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0.89070000000000005</v>
       </c>
@@ -5842,7 +5951,7 @@
         <v>0.42302543507362789</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0.98499999999999999</v>
       </c>
@@ -5869,8 +5978,12 @@
         <f t="shared" si="1"/>
         <v>0.27334732423924452</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53">
+        <f xml:space="preserve"> MAX(I53:I58)</f>
+        <v>0.28809283551967713</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0.87060000000000004</v>
       </c>
@@ -5898,7 +6011,7 @@
         <v>5.5304740406320545E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0.58250000000000002</v>
       </c>
@@ -5926,7 +6039,7 @@
         <v>0.15278884462151396</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0.19500000000000001</v>
       </c>
@@ -5940,6 +6053,10 @@
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
+      <c r="E56">
+        <f xml:space="preserve"> MIN(D56:D63)</f>
+        <v>0.28587962962962959</v>
+      </c>
       <c r="F56">
         <v>0.19819999999999999</v>
       </c>
@@ -5954,7 +6071,7 @@
         <v>0.28809283551967713</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>8.6400000000000005E-2</v>
       </c>
@@ -5982,7 +6099,7 @@
         <v>0.19047619047619047</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>8.1799999999999998E-2</v>
       </c>
@@ -6010,7 +6127,7 @@
         <v>0.28109965635738832</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3.3399999999999999E-2</v>
       </c>
@@ -6037,8 +6154,12 @@
         <f t="shared" si="1"/>
         <v>0.47011952191235057</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J59">
+        <f xml:space="preserve"> MIN(I59:I62)</f>
+        <v>0.32157394843962006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1.77E-2</v>
       </c>
@@ -6066,7 +6187,7 @@
         <v>0.44367816091954027</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -6094,7 +6215,7 @@
         <v>0.32157394843962006</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3.32E-2</v>
       </c>
@@ -6122,7 +6243,7 @@
         <v>0.45609318996415771</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1.5100000000000001E-2</v>
       </c>
@@ -6149,8 +6270,12 @@
         <f t="shared" si="1"/>
         <v>0.20066334991708126</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J63">
+        <f xml:space="preserve"> MAX(I63:I80,I81:I94)</f>
+        <v>0.43685914732865622</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>9.8599999999999993E-2</v>
       </c>
@@ -6162,6 +6287,10 @@
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
+        <v>0.38133874239350918</v>
+      </c>
+      <c r="E64">
+        <f xml:space="preserve"> MAX(D64:D75)</f>
         <v>0.38133874239350918</v>
       </c>
       <c r="F64">
@@ -6500,6 +6629,10 @@
         <f t="shared" si="2"/>
         <v>0.4949324324324324</v>
       </c>
+      <c r="E76">
+        <f xml:space="preserve"> MIN(D76:D78)</f>
+        <v>0.47692307692307695</v>
+      </c>
       <c r="F76">
         <v>0.41510000000000002</v>
       </c>
@@ -6584,6 +6717,10 @@
         <f t="shared" si="2"/>
         <v>0.303975058456742</v>
       </c>
+      <c r="E79">
+        <f xml:space="preserve"> MAX(D79:D80)</f>
+        <v>0.303975058456742</v>
+      </c>
       <c r="F79">
         <v>0.32250000000000001</v>
       </c>
@@ -6626,7 +6763,7 @@
         <v>0.23057851239669422</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>3.44E-2</v>
       </c>
@@ -6640,6 +6777,10 @@
         <f t="shared" si="2"/>
         <v>0.47093023255813948</v>
       </c>
+      <c r="E81">
+        <f xml:space="preserve"> MIN(D81:D82)</f>
+        <v>0.47093023255813948</v>
+      </c>
       <c r="F81">
         <v>0.21360000000000001</v>
       </c>
@@ -6654,7 +6795,7 @@
         <v>0.2092696629213483</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1.7399999999999999E-2</v>
       </c>
@@ -6682,7 +6823,7 @@
         <v>0.22004454342984409</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0.28710000000000002</v>
       </c>
@@ -6696,6 +6837,10 @@
         <f t="shared" si="2"/>
         <v>0.30929989550679204</v>
       </c>
+      <c r="E83">
+        <f xml:space="preserve"> MAX(D83:D86)</f>
+        <v>0.4642032332563511</v>
+      </c>
       <c r="F83">
         <v>8.8499999999999995E-2</v>
       </c>
@@ -6710,7 +6855,7 @@
         <v>0.38757062146892657</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0.16120000000000001</v>
       </c>
@@ -6738,7 +6883,7 @@
         <v>0.17557251908396945</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0.21390000000000001</v>
       </c>
@@ -6766,7 +6911,7 @@
         <v>0.11149032992036403</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0.12989999999999999</v>
       </c>
@@ -6794,7 +6939,7 @@
         <v>0.43685914732865622</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2.1100000000000001E-2</v>
       </c>
@@ -6808,6 +6953,10 @@
         <f t="shared" si="2"/>
         <v>0.54502369668246442</v>
       </c>
+      <c r="E87">
+        <f xml:space="preserve"> MIN(D87:D91)</f>
+        <v>0.46753246753246752</v>
+      </c>
       <c r="F87">
         <v>0.39839999999999998</v>
       </c>
@@ -6822,7 +6971,7 @@
         <v>0.21059236947791166</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2.3099999999999999E-2</v>
       </c>
@@ -6850,7 +6999,7 @@
         <v>0.2657976763955795</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>3.0800000000000001E-2</v>
       </c>
@@ -6878,7 +7027,7 @@
         <v>0.16410256410256407</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2.8199999999999999E-2</v>
       </c>
@@ -6906,7 +7055,7 @@
         <v>0.14863102998696218</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>0.13150000000000001</v>
       </c>
@@ -6934,7 +7083,7 @@
         <v>0.15842349304482228</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0.47549999999999998</v>
       </c>
@@ -6948,6 +7097,10 @@
         <f t="shared" si="2"/>
         <v>0.11272344900105154</v>
       </c>
+      <c r="E92">
+        <f xml:space="preserve"> MAX(D92:D93)</f>
+        <v>0.15724244771494966</v>
+      </c>
       <c r="F92">
         <v>0.2104</v>
       </c>
@@ -6962,7 +7115,7 @@
         <v>0.15731939163498099</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0.38729999999999998</v>
       </c>
@@ -6990,7 +7143,7 @@
         <v>0.43523316062176165</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>3.2399999999999998E-2</v>
       </c>
@@ -7004,6 +7157,9 @@
         <f t="shared" si="2"/>
         <v>0.5864197530864198</v>
       </c>
+      <c r="E94">
+        <v>0.58642000000000005</v>
+      </c>
       <c r="F94">
         <v>0.10390000000000001</v>
       </c>
@@ -7018,7 +7174,7 @@
         <v>0.40423484119345526</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2.2599999999999999E-2</v>
       </c>
@@ -7032,6 +7188,10 @@
         <f t="shared" si="2"/>
         <v>0.41150442477876104</v>
       </c>
+      <c r="E95">
+        <f xml:space="preserve"> MIN(D95:D110)</f>
+        <v>0.26451612903225807</v>
+      </c>
       <c r="F95">
         <v>4.41E-2</v>
       </c>
@@ -7045,8 +7205,12 @@
         <f t="shared" si="3"/>
         <v>0.4399092970521542</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J95">
+        <f xml:space="preserve"> MIN(I95:I97)</f>
+        <v>0.4399092970521542</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2.86E-2</v>
       </c>
@@ -7074,7 +7238,7 @@
         <v>0.58529411764705885</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4.0800000000000003E-2</v>
       </c>
@@ -7102,7 +7266,7 @@
         <v>0.53150481838398822</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2.6700000000000002E-2</v>
       </c>
@@ -7129,8 +7293,12 @@
         <f t="shared" si="3"/>
         <v>0.44677137870855149</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J98">
+        <f xml:space="preserve"> MAX(I98:I99)</f>
+        <v>0.44677137870855149</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2.4500000000000001E-2</v>
       </c>
@@ -7158,7 +7326,7 @@
         <v>0.28824932895914107</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2.1899999999999999E-2</v>
       </c>
@@ -7185,8 +7353,12 @@
         <f t="shared" si="3"/>
         <v>0.5224839400428265</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J100">
+        <f xml:space="preserve"> MIN(I100:I105)</f>
+        <v>0.31826741996233515</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2.6200000000000001E-2</v>
       </c>
@@ -7214,7 +7386,7 @@
         <v>0.33381502890173409</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2.4199999999999999E-2</v>
       </c>
@@ -7242,7 +7414,7 @@
         <v>0.31826741996233515</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2.0899999999999998E-2</v>
       </c>
@@ -7270,7 +7442,7 @@
         <v>0.31942215088282505</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2.1700000000000001E-2</v>
       </c>
@@ -7298,7 +7470,7 @@
         <v>0.33391304347826084</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2.7199999999999998E-2</v>
       </c>
@@ -7326,7 +7498,7 @@
         <v>0.39226519337016574</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2.7799999999999998E-2</v>
       </c>
@@ -7353,8 +7525,12 @@
         <f t="shared" si="3"/>
         <v>0.47111111111111109</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J106">
+        <f xml:space="preserve"> MAX(I106:I111)</f>
+        <v>0.47111111111111109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2.8000000000000001E-2</v>
       </c>
@@ -7382,7 +7558,7 @@
         <v>0.29201101928374656</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>4.65E-2</v>
       </c>
@@ -7410,7 +7586,7 @@
         <v>0.10096153846153846</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>3.49E-2</v>
       </c>
@@ -7438,7 +7614,7 @@
         <v>0.17662263067202758</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>3.2899999999999999E-2</v>
       </c>
@@ -7466,7 +7642,7 @@
         <v>0.11830303030303031</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F111">
         <v>0.45669999999999999</v>
       </c>
@@ -7481,7 +7657,7 @@
         <v>0.18108167287059337</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F112">
         <v>0.14879999999999999</v>
       </c>
@@ -7495,14 +7671,20 @@
         <f t="shared" si="3"/>
         <v>0.47513440860215056</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J112">
+        <f xml:space="preserve"> MIN(I112:I117)</f>
+        <v>0.33468559837728201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>13</v>
-      </c>
-      <c r="B113" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
       <c r="F113">
         <v>4.9299999999999997E-2</v>
       </c>
@@ -7517,7 +7699,7 @@
         <v>0.33468559837728201</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F114">
         <v>0.1983</v>
       </c>
@@ -7532,7 +7714,7 @@
         <v>0.45990922844175491</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F115">
         <v>0.53779999999999994</v>
       </c>
@@ -7547,7 +7729,7 @@
         <v>0.36110078095946452</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F116">
         <v>0.93659999999999999</v>
       </c>
@@ -7562,7 +7744,7 @@
         <v>0.39899636984838777</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F117">
         <v>0.32650000000000001</v>
       </c>
@@ -7577,7 +7759,7 @@
         <v>0.48514548238897398</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F118">
         <v>0.28360000000000002</v>
       </c>
@@ -7591,8 +7773,12 @@
         <f t="shared" si="3"/>
         <v>0.3236953455571227</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J118">
+        <f xml:space="preserve"> MAX(I118:I119)</f>
+        <v>0.32824686334350628</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F119">
         <v>0.2949</v>
       </c>
@@ -7607,7 +7793,7 @@
         <v>0.32824686334350628</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F120">
         <v>6.5500000000000003E-2</v>
       </c>
@@ -7621,8 +7807,12 @@
         <f t="shared" si="3"/>
         <v>0.45648854961832058</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J120">
+        <f xml:space="preserve"> MIN(I120:I130,I131:I140)</f>
+        <v>0.33123028391167197</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F121">
         <v>3.1E-2</v>
       </c>
@@ -7637,7 +7827,7 @@
         <v>0.54193548387096768</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F122">
         <v>3.1899999999999998E-2</v>
       </c>
@@ -7652,7 +7842,7 @@
         <v>0.40125391849529785</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F123">
         <v>2.87E-2</v>
       </c>
@@ -7667,7 +7857,7 @@
         <v>0.39372822299651566</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F124">
         <v>2.46E-2</v>
       </c>
@@ -7682,7 +7872,7 @@
         <v>0.52845528455284552</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F125">
         <v>2.4500000000000001E-2</v>
       </c>
@@ -7697,7 +7887,7 @@
         <v>0.45714285714285713</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F126">
         <v>2.5499999999999998E-2</v>
       </c>
@@ -7712,7 +7902,7 @@
         <v>0.48235294117647065</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F127">
         <v>2.3599999999999999E-2</v>
       </c>
@@ -7727,7 +7917,7 @@
         <v>0.53389830508474578</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F128">
         <v>2.4E-2</v>
       </c>
@@ -7926,14 +8116,18 @@
       <c r="F143" t="s">
         <v>11</v>
       </c>
-      <c r="G143" t="s">
-        <v>15</v>
-      </c>
+      <c r="G143" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="G143:I143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update time for fo
</commit_message>
<xml_diff>
--- a/ThongKeNguong.xlsx
+++ b/ThongKeNguong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Class\ky2_2122\XL tín hiệu số\Handle speech signal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F295D7B0-A7A8-4C83-A624-636D9CCD7F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE7927D-5800-432F-8B27-160E11AE7065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{4B47E6B4-FF19-4334-8229-3A9AFBCD530A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B47E6B4-FF19-4334-8229-3A9AFBCD530A}"/>
   </bookViews>
   <sheets>
     <sheet name="Studio" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF5C30D-5A8E-4793-A983-56FBF19A73A6}">
   <dimension ref="A1:S143"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100:C100"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4469,8 +4469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF1C9F2-E668-4C8F-9AA3-088A854E6FE4}">
   <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="J143" sqref="J143"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="G143" sqref="G143:I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>